<commit_message>
updated class diagram and prog specifications
</commit_message>
<xml_diff>
--- a/prove/Develop03/class_diagram.xlsx
+++ b/prove/Develop03/class_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\da\cse210\cse210-byu\prove\Develop03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC57145-CF45-43FA-AE8C-A81A502CDD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB38036-0FE2-4A89-AB29-430562014075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4593E8EE-613E-4214-9D7C-DAE1F7B07C1E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Class Program</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Class Word</t>
   </si>
   <si>
-    <t>HideWords()</t>
-  </si>
-  <si>
     <t>Reference()</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>_lastVerses: string</t>
   </si>
   <si>
-    <t>_hiddenWords: List&lt;string&gt;</t>
-  </si>
-  <si>
     <t>Main()</t>
   </si>
   <si>
@@ -92,19 +86,28 @@
     <t>GetReference():string</t>
   </si>
   <si>
-    <t>_words: string[]</t>
-  </si>
-  <si>
     <t>GetScripture()</t>
   </si>
   <si>
     <t>_word: List&lt;string&gt;</t>
   </si>
   <si>
-    <t>ReceiveWords()</t>
-  </si>
-  <si>
     <t>Display()</t>
+  </si>
+  <si>
+    <t>_words: List&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>SplitWords()</t>
+  </si>
+  <si>
+    <t>_hiddenWords: string</t>
+  </si>
+  <si>
+    <t>RandomWord()</t>
+  </si>
+  <si>
+    <t>EndGame()</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +554,7 @@
     </row>
     <row r="3" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -568,79 +571,80 @@
     </row>
     <row r="6" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>